<commit_message>
added number of new cases per week to excel
</commit_message>
<xml_diff>
--- a/new data for graph.xlsx
+++ b/new data for graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggary\Desktop\新增資料夾\Big-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\朱子赫\FCP\Big-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0E276D-0A46-4E26-AED6-7C1C8AA6EC8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2919F269-84E9-4D8A-84F5-A707D3FCAA83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="3630" windowWidth="21600" windowHeight="11385" xr2:uid="{1DA189A7-26AF-4824-A3C5-28F6646090FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1DA189A7-26AF-4824-A3C5-28F6646090FF}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Brain strom(Global, 国行)</t>
   </si>
@@ -61,6 +61,10 @@
     <t>得病的人数(当地)thousands</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>新增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -70,14 +74,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -111,7 +115,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -127,7 +131,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,13 +427,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE883F70-5F8C-4769-BAE9-FF5AFCBB3D4F}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -829,7 +833,7 @@
         <v>82.724999999999994</v>
       </c>
       <c r="C7">
-        <v>85.747</v>
+        <v>82.747</v>
       </c>
       <c r="D7">
         <v>82.759</v>
@@ -896,6 +900,106 @@
       </c>
       <c r="Y7">
         <v>82.957999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>C7*1000-B7*1000</f>
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:J8" si="0">D7*1000-C7*1000</f>
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8" si="1">K7*1000-J7*1000</f>
+        <v>27</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8" si="2">L7*1000-K7*1000</f>
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8" si="3">M7*1000-L7*1000</f>
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8" si="4">N7*1000-M7*1000</f>
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8" si="5">O7*1000-N7*1000</f>
+        <v>10</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:Q8" si="6">P7*1000-O7*1000</f>
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8" si="7">R7*1000-Q7*1000</f>
+        <v>22</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="S8" si="8">S7*1000-R7*1000</f>
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8" si="9">T7*1000-S7*1000</f>
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ref="U8" si="10">U7*1000-T7*1000</f>
+        <v>14</v>
+      </c>
+      <c r="V8">
+        <f t="shared" ref="V8" si="11">V7*1000-U7*1000</f>
+        <v>2</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ref="W8:X8" si="12">W7*1000-V7*1000</f>
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ref="Y8" si="13">Y7*1000-X7*1000</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed together, add gui
</commit_message>
<xml_diff>
--- a/new data for graph.xlsx
+++ b/new data for graph.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\朱子赫\FCP\Big-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jelly Jinzhe Liu\Desktop\Big-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2919F269-84E9-4D8A-84F5-A707D3FCAA83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D562CB0-A692-4CBD-8A60-1BAEA4108A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1DA189A7-26AF-4824-A3C5-28F6646090FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DA189A7-26AF-4824-A3C5-28F6646090FF}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -36,52 +36,46 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Brain strom(Global, 国行)</t>
+    <t>date</t>
   </si>
   <si>
-    <t>日期</t>
+    <t>Load factor</t>
   </si>
   <si>
-    <t>资金(入)billion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Outcome</t>
   </si>
   <si>
-    <t>客座率%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Income</t>
   </si>
   <si>
-    <t>资金(出)billion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Numbers of airplane(work)</t>
   </si>
   <si>
-    <t>天上飞的机数 thousands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Number of patients</t>
   </si>
   <si>
-    <t>得病的人数(当地)thousands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>New</t>
   </si>
   <si>
-    <t>新增</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Data of China airline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -429,20 +423,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE883F70-5F8C-4769-BAE9-FF5AFCBB3D4F}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>1.1000000000000001</v>
@@ -517,9 +509,9 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>29.2</v>
@@ -594,9 +586,9 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>76.599999999999994</v>
@@ -671,9 +663,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -748,9 +740,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>148.97</v>
@@ -825,9 +817,9 @@
         <v>109.02</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>82.724999999999994</v>
@@ -902,9 +894,9 @@
         <v>82.957999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>

</xml_diff>